<commit_message>
Final updates: IP block fix, timestamped report, QR rules
</commit_message>
<xml_diff>
--- a/student_list.xlsx
+++ b/student_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">roll </t>
   </si>
@@ -38,6 +38,18 @@
   </si>
   <si>
     <t>Priya Kapoor</t>
+  </si>
+  <si>
+    <t>23BCA004</t>
+  </si>
+  <si>
+    <t>Drishti paras</t>
+  </si>
+  <si>
+    <t>23BCA005</t>
+  </si>
+  <si>
+    <t>Ishan sharma</t>
   </si>
 </sst>
 </file>
@@ -384,7 +396,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -426,6 +438,22 @@
         <v>7</v>
       </c>
     </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>